<commit_message>
Add tip for canvas
</commit_message>
<xml_diff>
--- a/Tips web studio.xlsx
+++ b/Tips web studio.xlsx
@@ -5,13 +5,15 @@
   <sheets>
     <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1011</definedName>
+  </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="168">
   <si>
     <t>Ignored functional key</t>
   </si>
@@ -490,6 +492,9 @@
 Note that the WebForm is a component itself.</t>
   </si>
   <si>
+    <t>https://www.youtube.com/embed/MnyFw6O4B1M</t>
+  </si>
+  <si>
     <t>Show how to drag and drop a component
  Show the main tips (move, remove, duplicate, go to parent)
  Show the rendering</t>
@@ -499,9 +504,6 @@
   </si>
   <si>
     <t>editors:webform:datatablesetup</t>
-  </si>
-  <si>
-    <t>texttext</t>
   </si>
   <si>
     <t xml:space="preserve">**The datatable - A component to iterate on an entity selection** 
@@ -662,7 +664,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -736,6 +738,10 @@
     </font>
     <font>
       <u/>
+      <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12.0"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
@@ -766,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -867,16 +873,19 @@
     <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2562,9 +2571,14 @@
       <c r="E36" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="25"/>
-      <c r="H36" s="34" t="s">
+      <c r="F36" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>127</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>128</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2590,20 +2604,20 @@
     </row>
     <row r="37">
       <c r="A37" s="25" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B37" s="8"/>
       <c r="C37" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>130</v>
+      <c r="D37" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>131</v>
       </c>
       <c r="G37" s="25"/>
-      <c r="H37" s="34" t="s">
+      <c r="H37" s="35" t="s">
         <v>132</v>
       </c>
       <c r="I37" s="8"/>
@@ -2684,13 +2698,13 @@
       </c>
       <c r="F39" s="29"/>
       <c r="G39" s="25"/>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="35" t="s">
         <v>140</v>
       </c>
       <c r="I39" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="J39" s="35"/>
+      <c r="J39" s="36"/>
       <c r="K39" s="11"/>
       <c r="L39" s="11"/>
       <c r="M39" s="8"/>
@@ -2727,9 +2741,9 @@
       </c>
       <c r="F40" s="29"/>
       <c r="G40" s="25"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="38"/>
       <c r="K40" s="11"/>
       <c r="L40" s="11"/>
       <c r="M40" s="8"/>
@@ -2766,11 +2780,11 @@
       </c>
       <c r="F41" s="29"/>
       <c r="G41" s="25"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37" t="s">
+      <c r="H41" s="37"/>
+      <c r="I41" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="J41" s="37" t="s">
+      <c r="J41" s="38" t="s">
         <v>149</v>
       </c>
       <c r="K41" s="11"/>
@@ -2812,8 +2826,8 @@
       <c r="H42" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="I42" s="35"/>
-      <c r="J42" s="35"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
       <c r="K42" s="11"/>
       <c r="L42" s="11"/>
       <c r="M42" s="8"/>
@@ -2856,7 +2870,7 @@
       <c r="I43" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="J43" s="35"/>
+      <c r="J43" s="36"/>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
       <c r="M43" s="8"/>
@@ -2896,8 +2910,8 @@
       <c r="H44" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
       <c r="M44" s="8"/>
@@ -2934,7 +2948,7 @@
       </c>
       <c r="F45" s="29"/>
       <c r="G45" s="25"/>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="35" t="s">
         <v>166</v>
       </c>
       <c r="I45" s="25" t="s">
@@ -32908,6 +32922,7 @@
       <c r="AC1011" s="8"/>
     </row>
   </sheetData>
+  <autoFilter ref="$D$1:$D$1011"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G7"/>
     <hyperlink r:id="rId2" ref="G8"/>
@@ -32917,9 +32932,10 @@
     <hyperlink r:id="rId6" ref="G25"/>
     <hyperlink r:id="rId7" ref="G27"/>
     <hyperlink r:id="rId8" ref="G29"/>
-    <hyperlink r:id="rId9" ref="I41"/>
-    <hyperlink r:id="rId10" ref="J41"/>
+    <hyperlink r:id="rId9" ref="G36"/>
+    <hyperlink r:id="rId10" ref="I41"/>
+    <hyperlink r:id="rId11" ref="J41"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update tips canvas + style library (2)
</commit_message>
<xml_diff>
--- a/Tips web studio.xlsx
+++ b/Tips web studio.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Feuille 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1011</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1015</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="170">
   <si>
     <t>Ignored functional key</t>
   </si>
@@ -206,6 +206,9 @@
     <t>https://www.youtube.com/embed/K0SrUOS7LB8</t>
   </si>
   <si>
+    <t>https://www.youtube.com/embed/4ILg3uIeF-U</t>
+  </si>
+  <si>
     <t>Button</t>
   </si>
   <si>
@@ -228,7 +231,7 @@
   </si>
   <si>
     <t>**Radio button - Select values among a list**
-The radio button is a component to select one or several value among a given list.</t>
+The radio button is a component to select one or several values among a given list.</t>
   </si>
   <si>
     <t>Show how to set the options values
@@ -472,6 +475,9 @@
 They can be applied by drag and drop on the component or using the properties panel.</t>
   </si>
   <si>
+    <t>https://www.youtube.com/embed/z_1A6roVlgk</t>
+  </si>
+  <si>
     <t>Show how to create a new css (show the CSS code editor) and apply it on a component
  Show to export styles applied on a component in a new css
  Show how to apply a CSS on a component</t>
@@ -664,7 +670,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -709,6 +715,19 @@
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
     </font>
     <font>
@@ -719,15 +738,6 @@
       <u/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF1155CC"/>
     </font>
     <font/>
     <font>
@@ -772,7 +782,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -828,6 +838,16 @@
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -837,55 +857,52 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1708,24 +1725,24 @@
       <c r="AC14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="19"/>
+      <c r="C15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="H15" s="7"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -1749,23 +1766,23 @@
       <c r="AC15" s="8"/>
     </row>
     <row r="16">
-      <c r="A16" s="19" t="s">
-        <v>57</v>
+      <c r="A16" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="14" t="s">
-        <v>58</v>
+      <c r="C16" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="11"/>
       <c r="H16" s="7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
@@ -1790,24 +1807,24 @@
       <c r="AC16" s="8"/>
     </row>
     <row r="17">
-      <c r="A17" s="19" t="s">
-        <v>57</v>
+      <c r="A17" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="17" t="s">
-        <v>31</v>
+      <c r="E17" s="20" t="s">
+        <v>60</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="F17" s="8"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="H17" s="7"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -1831,24 +1848,24 @@
       <c r="AC17" s="8"/>
     </row>
     <row r="18">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="7" t="s">
-        <v>65</v>
-      </c>
+      <c r="H18" s="7"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -1872,23 +1889,23 @@
       <c r="AC18" s="8"/>
     </row>
     <row r="19">
-      <c r="A19" s="19" t="s">
-        <v>66</v>
+      <c r="A19" s="23" t="s">
+        <v>63</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="11"/>
       <c r="H19" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
@@ -1900,7 +1917,7 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="20"/>
+      <c r="S19" s="8"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
@@ -1913,23 +1930,23 @@
       <c r="AC19" s="8"/>
     </row>
     <row r="20">
-      <c r="A20" s="19" t="s">
-        <v>69</v>
+      <c r="A20" s="23" t="s">
+        <v>67</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="11"/>
       <c r="H20" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
@@ -1941,7 +1958,7 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
+      <c r="S20" s="24"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
@@ -1954,23 +1971,23 @@
       <c r="AC20" s="8"/>
     </row>
     <row r="21">
-      <c r="A21" s="19" t="s">
-        <v>73</v>
+      <c r="A21" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>75</v>
+      <c r="E21" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="11"/>
       <c r="H21" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
@@ -1995,23 +2012,23 @@
       <c r="AC21" s="8"/>
     </row>
     <row r="22">
-      <c r="A22" s="19" t="s">
-        <v>77</v>
+      <c r="A22" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>79</v>
+      <c r="E22" s="25" t="s">
+        <v>76</v>
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="11"/>
       <c r="H22" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
@@ -2036,23 +2053,23 @@
       <c r="AC22" s="8"/>
     </row>
     <row r="23">
-      <c r="A23" s="19" t="s">
-        <v>81</v>
+      <c r="A23" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="11"/>
       <c r="H23" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
@@ -2077,22 +2094,24 @@
       <c r="AC23" s="8"/>
     </row>
     <row r="24">
-      <c r="A24" s="19" t="s">
-        <v>85</v>
+      <c r="A24" s="23" t="s">
+        <v>82</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -2116,28 +2135,22 @@
       <c r="AC24" s="8"/>
     </row>
     <row r="25">
-      <c r="A25" s="19" t="s">
-        <v>85</v>
+      <c r="A25" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>90</v>
-      </c>
+      <c r="F25" s="26"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="7"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -2161,23 +2174,27 @@
       <c r="AC25" s="8"/>
     </row>
     <row r="26">
-      <c r="A26" s="19" t="s">
-        <v>91</v>
+      <c r="A26" s="23" t="s">
+        <v>86</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="11"/>
+      <c r="F26" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>90</v>
+      </c>
       <c r="H26" s="7" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
@@ -2202,24 +2219,24 @@
       <c r="AC26" s="8"/>
     </row>
     <row r="27">
-      <c r="A27" s="19" t="s">
-        <v>91</v>
+      <c r="A27" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="23" t="s">
-        <v>31</v>
+      <c r="E27" s="7" t="s">
+        <v>94</v>
       </c>
-      <c r="G27" s="26" t="s">
+      <c r="F27" s="25"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="H27" s="25"/>
       <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
@@ -2243,20 +2260,24 @@
       <c r="AC27" s="8"/>
     </row>
     <row r="28">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="29"/>
+      <c r="F28" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="25"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
@@ -2281,23 +2302,19 @@
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
-      <c r="D29" s="15" t="s">
-        <v>30</v>
+      <c r="D29" s="5" t="s">
+        <v>11</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" s="26" t="s">
+      <c r="E29" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="25"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
@@ -2322,23 +2339,23 @@
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="25" t="s">
-        <v>103</v>
-      </c>
+      <c r="H30" s="29"/>
       <c r="I30" s="8"/>
       <c r="J30" s="8"/>
       <c r="K30" s="8"/>
@@ -2362,20 +2379,24 @@
       <c r="AC30" s="8"/>
     </row>
     <row r="31">
-      <c r="A31" s="28" t="s">
-        <v>104</v>
+      <c r="A31" s="6" t="s">
+        <v>101</v>
       </c>
+      <c r="B31" s="8"/>
       <c r="C31" s="6" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="25" t="s">
-        <v>106</v>
+      <c r="E31" s="29" t="s">
+        <v>103</v>
       </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="29" t="s">
+        <v>104</v>
+      </c>
       <c r="I31" s="8"/>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
@@ -2399,22 +2420,20 @@
       <c r="AC31" s="8"/>
     </row>
     <row r="32">
-      <c r="A32" s="28" t="s">
-        <v>107</v>
+      <c r="A32" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="25" t="s">
-        <v>109</v>
+      <c r="E32" s="29" t="s">
+        <v>107</v>
       </c>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25" t="s">
-        <v>110</v>
-      </c>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
@@ -2438,21 +2457,21 @@
       <c r="AC32" s="8"/>
     </row>
     <row r="33">
-      <c r="A33" s="30" t="s">
-        <v>111</v>
+      <c r="A33" s="21" t="s">
+        <v>108</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="31" t="s">
-        <v>113</v>
+      <c r="E33" s="29" t="s">
+        <v>110</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31" t="s">
-        <v>114</v>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29" t="s">
+        <v>111</v>
       </c>
       <c r="I33" s="8"/>
       <c r="J33" s="8"/>
@@ -2478,20 +2497,20 @@
     </row>
     <row r="34">
       <c r="A34" s="32" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="25" t="s">
-        <v>117</v>
+      <c r="E34" s="33" t="s">
+        <v>114</v>
       </c>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25" t="s">
-        <v>118</v>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
@@ -2515,27 +2534,24 @@
       <c r="AB34" s="8"/>
       <c r="AC34" s="8"/>
     </row>
-    <row r="35" ht="105.75" customHeight="1">
-      <c r="A35" s="32" t="s">
-        <v>119</v>
+    <row r="35">
+      <c r="A35" s="34" t="s">
+        <v>116</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="25" t="s">
-        <v>121</v>
+      <c r="E35" s="29" t="s">
+        <v>118</v>
       </c>
-      <c r="F35" s="28"/>
       <c r="G35" s="29"/>
-      <c r="H35" s="25" t="s">
-        <v>122</v>
+      <c r="H35" s="29" t="s">
+        <v>119</v>
       </c>
-      <c r="I35" s="33" t="s">
-        <v>123</v>
-      </c>
+      <c r="I35" s="8"/>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
       <c r="L35" s="8"/>
@@ -2557,70 +2573,67 @@
       <c r="AB35" s="8"/>
       <c r="AC35" s="8"/>
     </row>
-    <row r="36">
-      <c r="A36" s="32" t="s">
+    <row r="36" ht="105.75" customHeight="1">
+      <c r="A36" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="21"/>
+      <c r="G36" s="35"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="19"/>
+      <c r="Z36" s="19"/>
+      <c r="AA36" s="19"/>
+      <c r="AB36" s="19"/>
+      <c r="AC36" s="19"/>
+    </row>
+    <row r="37" ht="105.75" customHeight="1">
+      <c r="A37" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="6" t="s">
+      <c r="I37" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="F36" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>127</v>
-      </c>
-      <c r="H36" s="35" t="s">
-        <v>128</v>
-      </c>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="8"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="8"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
-      <c r="AC36" s="8"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="G37" s="25"/>
-      <c r="H37" s="35" t="s">
-        <v>132</v>
-      </c>
-      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -2642,110 +2655,113 @@
       <c r="AB37" s="8"/>
       <c r="AC37" s="8"/>
     </row>
-    <row r="38">
-      <c r="A38" s="32" t="s">
-        <v>133</v>
+    <row r="38" ht="105.75" customHeight="1">
+      <c r="A38" s="34" t="s">
+        <v>120</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="6" t="s">
-        <v>134</v>
+      <c r="C38" s="14" t="s">
+        <v>121</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="H38" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="I38" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
+      <c r="Y38" s="19"/>
+      <c r="Z38" s="19"/>
+      <c r="AA38" s="19"/>
+      <c r="AB38" s="19"/>
+      <c r="AC38" s="19"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E38" s="25" t="s">
-        <v>135</v>
+      <c r="E39" s="29" t="s">
+        <v>128</v>
       </c>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25" t="s">
-        <v>136</v>
+      <c r="G39" s="37"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
+      <c r="Y39" s="19"/>
+      <c r="Z39" s="19"/>
+      <c r="AA39" s="19"/>
+      <c r="AB39" s="19"/>
+      <c r="AC39" s="19"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="34" t="s">
+        <v>126</v>
       </c>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-      <c r="AA38" s="8"/>
-      <c r="AB38" s="8"/>
-      <c r="AC38" s="8"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="25" t="s">
-        <v>137</v>
+      <c r="B40" s="8"/>
+      <c r="C40" s="6" t="s">
+        <v>127</v>
       </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="6" t="s">
-        <v>138</v>
+      <c r="D40" s="15" t="s">
+        <v>30</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>11</v>
+      <c r="E40" s="29"/>
+      <c r="F40" s="27" t="s">
+        <v>31</v>
       </c>
-      <c r="E39" s="25" t="s">
-        <v>139</v>
+      <c r="G40" s="37" t="s">
+        <v>129</v>
       </c>
-      <c r="F39" s="29"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="35" t="s">
-        <v>140</v>
+      <c r="H40" s="38" t="s">
+        <v>130</v>
       </c>
-      <c r="I39" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="J39" s="36"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-      <c r="O39" s="8"/>
-      <c r="P39" s="8"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
-      <c r="AB39" s="8"/>
-      <c r="AC39" s="8"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="B40" s="11"/>
-      <c r="C40" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F40" s="29"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+      <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
       <c r="O40" s="8"/>
@@ -2765,30 +2781,27 @@
       <c r="AC40" s="8"/>
     </row>
     <row r="41">
-      <c r="A41" s="25" t="s">
-        <v>145</v>
+      <c r="A41" s="29" t="s">
+        <v>131</v>
       </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="4" t="s">
-        <v>146</v>
+      <c r="B41" s="8"/>
+      <c r="C41" s="6" t="s">
+        <v>132</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E41" s="25" t="s">
-        <v>147</v>
+      <c r="E41" s="29" t="s">
+        <v>133</v>
       </c>
-      <c r="F41" s="29"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="37"/>
-      <c r="I41" s="38" t="s">
-        <v>148</v>
+      <c r="G41" s="29"/>
+      <c r="H41" s="38" t="s">
+        <v>134</v>
       </c>
-      <c r="J41" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
       <c r="O41" s="8"/>
@@ -2808,28 +2821,27 @@
       <c r="AC41" s="8"/>
     </row>
     <row r="42">
-      <c r="A42" s="25" t="s">
-        <v>150</v>
+      <c r="A42" s="34" t="s">
+        <v>135</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="4" t="s">
-        <v>151</v>
+      <c r="B42" s="8"/>
+      <c r="C42" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E42" s="25" t="s">
-        <v>152</v>
+      <c r="E42" s="29" t="s">
+        <v>137</v>
       </c>
-      <c r="F42" s="29"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25" t="s">
-        <v>153</v>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29" t="s">
+        <v>138</v>
       </c>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+      <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
       <c r="O42" s="8"/>
@@ -2849,28 +2861,28 @@
       <c r="AC42" s="8"/>
     </row>
     <row r="43">
-      <c r="A43" s="25" t="s">
-        <v>154</v>
+      <c r="A43" s="29" t="s">
+        <v>139</v>
       </c>
       <c r="B43" s="11"/>
-      <c r="C43" s="4" t="s">
-        <v>155</v>
+      <c r="C43" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E43" s="25" t="s">
-        <v>156</v>
+      <c r="E43" s="29" t="s">
+        <v>141</v>
       </c>
-      <c r="F43" s="29"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25" t="s">
-        <v>157</v>
+      <c r="F43" s="31"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="38" t="s">
+        <v>142</v>
       </c>
-      <c r="I43" s="25" t="s">
-        <v>158</v>
+      <c r="I43" s="29" t="s">
+        <v>143</v>
       </c>
-      <c r="J43" s="36"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="11"/>
       <c r="L43" s="11"/>
       <c r="M43" s="8"/>
@@ -2892,26 +2904,24 @@
       <c r="AC43" s="8"/>
     </row>
     <row r="44">
-      <c r="A44" s="25" t="s">
-        <v>159</v>
+      <c r="A44" s="29" t="s">
+        <v>144</v>
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="4" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="25" t="s">
-        <v>161</v>
+      <c r="E44" s="29" t="s">
+        <v>146</v>
       </c>
-      <c r="F44" s="29"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25" t="s">
-        <v>162</v>
-      </c>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
       <c r="M44" s="8"/>
@@ -2933,28 +2943,28 @@
       <c r="AC44" s="8"/>
     </row>
     <row r="45">
-      <c r="A45" s="25" t="s">
-        <v>163</v>
+      <c r="A45" s="29" t="s">
+        <v>147</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="4" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E45" s="25" t="s">
-        <v>165</v>
+      <c r="E45" s="29" t="s">
+        <v>149</v>
       </c>
-      <c r="F45" s="29"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="35" t="s">
-        <v>166</v>
+      <c r="F45" s="31"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41" t="s">
+        <v>150</v>
       </c>
-      <c r="I45" s="25" t="s">
-        <v>167</v>
+      <c r="J45" s="41" t="s">
+        <v>151</v>
       </c>
-      <c r="J45" s="11"/>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="8"/>
@@ -2976,18 +2986,28 @@
       <c r="AC45" s="8"/>
     </row>
     <row r="46">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
+      <c r="A46" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F46" s="31"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
       <c r="O46" s="8"/>
@@ -3007,18 +3027,30 @@
       <c r="AC46" s="8"/>
     </row>
     <row r="47">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
+      <c r="A47" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="F47" s="31"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="I47" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="J47" s="39"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
       <c r="O47" s="8"/>
@@ -3038,18 +3070,28 @@
       <c r="AC47" s="8"/>
     </row>
     <row r="48">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
+      <c r="A48" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="F48" s="31"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
       <c r="O48" s="8"/>
@@ -3069,18 +3111,30 @@
       <c r="AC48" s="8"/>
     </row>
     <row r="49">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="8"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="8"/>
+      <c r="A49" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E49" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" s="31"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="I49" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="11"/>
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
       <c r="O49" s="8"/>
@@ -32921,21 +32975,148 @@
       <c r="AB1011" s="8"/>
       <c r="AC1011" s="8"/>
     </row>
+    <row r="1012">
+      <c r="A1012" s="8"/>
+      <c r="B1012" s="8"/>
+      <c r="C1012" s="8"/>
+      <c r="D1012" s="8"/>
+      <c r="E1012" s="8"/>
+      <c r="F1012" s="8"/>
+      <c r="G1012" s="11"/>
+      <c r="H1012" s="11"/>
+      <c r="I1012" s="8"/>
+      <c r="J1012" s="8"/>
+      <c r="K1012" s="8"/>
+      <c r="L1012" s="8"/>
+      <c r="M1012" s="8"/>
+      <c r="N1012" s="8"/>
+      <c r="O1012" s="8"/>
+      <c r="P1012" s="8"/>
+      <c r="Q1012" s="8"/>
+      <c r="R1012" s="8"/>
+      <c r="S1012" s="8"/>
+      <c r="T1012" s="8"/>
+      <c r="U1012" s="8"/>
+      <c r="V1012" s="8"/>
+      <c r="W1012" s="8"/>
+      <c r="X1012" s="8"/>
+      <c r="Y1012" s="8"/>
+      <c r="Z1012" s="8"/>
+      <c r="AA1012" s="8"/>
+      <c r="AB1012" s="8"/>
+      <c r="AC1012" s="8"/>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="8"/>
+      <c r="B1013" s="8"/>
+      <c r="C1013" s="8"/>
+      <c r="D1013" s="8"/>
+      <c r="E1013" s="8"/>
+      <c r="F1013" s="8"/>
+      <c r="G1013" s="11"/>
+      <c r="H1013" s="11"/>
+      <c r="I1013" s="8"/>
+      <c r="J1013" s="8"/>
+      <c r="K1013" s="8"/>
+      <c r="L1013" s="8"/>
+      <c r="M1013" s="8"/>
+      <c r="N1013" s="8"/>
+      <c r="O1013" s="8"/>
+      <c r="P1013" s="8"/>
+      <c r="Q1013" s="8"/>
+      <c r="R1013" s="8"/>
+      <c r="S1013" s="8"/>
+      <c r="T1013" s="8"/>
+      <c r="U1013" s="8"/>
+      <c r="V1013" s="8"/>
+      <c r="W1013" s="8"/>
+      <c r="X1013" s="8"/>
+      <c r="Y1013" s="8"/>
+      <c r="Z1013" s="8"/>
+      <c r="AA1013" s="8"/>
+      <c r="AB1013" s="8"/>
+      <c r="AC1013" s="8"/>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="8"/>
+      <c r="B1014" s="8"/>
+      <c r="C1014" s="8"/>
+      <c r="D1014" s="8"/>
+      <c r="E1014" s="8"/>
+      <c r="F1014" s="8"/>
+      <c r="G1014" s="11"/>
+      <c r="H1014" s="11"/>
+      <c r="I1014" s="8"/>
+      <c r="J1014" s="8"/>
+      <c r="K1014" s="8"/>
+      <c r="L1014" s="8"/>
+      <c r="M1014" s="8"/>
+      <c r="N1014" s="8"/>
+      <c r="O1014" s="8"/>
+      <c r="P1014" s="8"/>
+      <c r="Q1014" s="8"/>
+      <c r="R1014" s="8"/>
+      <c r="S1014" s="8"/>
+      <c r="T1014" s="8"/>
+      <c r="U1014" s="8"/>
+      <c r="V1014" s="8"/>
+      <c r="W1014" s="8"/>
+      <c r="X1014" s="8"/>
+      <c r="Y1014" s="8"/>
+      <c r="Z1014" s="8"/>
+      <c r="AA1014" s="8"/>
+      <c r="AB1014" s="8"/>
+      <c r="AC1014" s="8"/>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="8"/>
+      <c r="B1015" s="8"/>
+      <c r="C1015" s="8"/>
+      <c r="D1015" s="8"/>
+      <c r="E1015" s="8"/>
+      <c r="F1015" s="8"/>
+      <c r="G1015" s="11"/>
+      <c r="H1015" s="11"/>
+      <c r="I1015" s="8"/>
+      <c r="J1015" s="8"/>
+      <c r="K1015" s="8"/>
+      <c r="L1015" s="8"/>
+      <c r="M1015" s="8"/>
+      <c r="N1015" s="8"/>
+      <c r="O1015" s="8"/>
+      <c r="P1015" s="8"/>
+      <c r="Q1015" s="8"/>
+      <c r="R1015" s="8"/>
+      <c r="S1015" s="8"/>
+      <c r="T1015" s="8"/>
+      <c r="U1015" s="8"/>
+      <c r="V1015" s="8"/>
+      <c r="W1015" s="8"/>
+      <c r="X1015" s="8"/>
+      <c r="Y1015" s="8"/>
+      <c r="Z1015" s="8"/>
+      <c r="AA1015" s="8"/>
+      <c r="AB1015" s="8"/>
+      <c r="AC1015" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$D$1:$D$1011"/>
+  <autoFilter ref="$D$1:$D$1015"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G7"/>
     <hyperlink r:id="rId2" ref="G8"/>
     <hyperlink r:id="rId3" ref="G13"/>
     <hyperlink r:id="rId4" ref="G14"/>
-    <hyperlink r:id="rId5" ref="G17"/>
-    <hyperlink r:id="rId6" ref="G25"/>
-    <hyperlink r:id="rId7" ref="G27"/>
-    <hyperlink r:id="rId8" ref="G29"/>
-    <hyperlink r:id="rId9" ref="G36"/>
-    <hyperlink r:id="rId10" ref="I41"/>
-    <hyperlink r:id="rId11" ref="J41"/>
+    <hyperlink r:id="rId5" ref="G15"/>
+    <hyperlink r:id="rId6" ref="G18"/>
+    <hyperlink r:id="rId7" ref="G26"/>
+    <hyperlink r:id="rId8" ref="G28"/>
+    <hyperlink r:id="rId9" ref="G30"/>
+    <hyperlink r:id="rId10" ref="G37"/>
+    <hyperlink r:id="rId11" ref="G38"/>
+    <hyperlink r:id="rId12" ref="G40"/>
+    <hyperlink r:id="rId13" ref="I45"/>
+    <hyperlink r:id="rId14" ref="J45"/>
   </hyperlinks>
-  <drawing r:id="rId12"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add tip remote datasource
</commit_message>
<xml_diff>
--- a/Tips web studio.xlsx
+++ b/Tips web studio.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="Feuille 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1015</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1016</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="174">
   <si>
     <t>Ignored functional key</t>
   </si>
@@ -447,6 +447,18 @@
     </r>
   </si>
   <si>
+    <t>editors:webform:toolbox:datasources:remote</t>
+  </si>
+  <si>
+    <t>**Remote datasources - Handle data on the server**
+Remote datasources are [entities](https://developer.4d.com/docs/en/ORDA/dsmapping.html#entity) and e[ntity selections](https://developer.4d.com/docs/en/ORDA/dsmapping.html#entity-selection).
+They are handled on the server and can be assigned to components. They offer functions defined on the ORDA classes that they instantiate ([Entity class](https://developer.4d.com/docs/en/ORDA/ordaClasses.html#entity-class), [Entity Selection class](https://developer.4d.com/docs/en/ORDA/ordaClasses.html#entityselection-class)).
+[Visit the documentation to learn more](https://developer.4d.com/4d-web-studio/docs/datasources/) and watch the tips.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/fCS0RYyx0p8</t>
+  </si>
+  <si>
     <t>Catalog</t>
   </si>
   <si>
@@ -464,9 +476,6 @@
   </si>
   <si>
     <t>Remote</t>
-  </si>
-  <si>
-    <t>editors:webform:toolbox:datasources:remote</t>
   </si>
   <si>
     <t>**Remote datasources - The data persisted in your database**
@@ -697,7 +706,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -766,6 +775,11 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <u/>
+      <color rgb="FF1155CC"/>
+      <name val="&quot;Arial&quot;"/>
+    </font>
+    <font>
       <b/>
       <sz val="12.0"/>
       <color rgb="FF000000"/>
@@ -812,7 +826,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -895,6 +909,12 @@
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
@@ -907,22 +927,22 @@
     <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2520,23 +2540,26 @@
       <c r="AB33" s="8"/>
       <c r="AC33" s="8"/>
     </row>
-    <row r="34">
+    <row r="34" ht="273.0" customHeight="1">
       <c r="A34" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24" t="s">
-        <v>115</v>
-      </c>
+      <c r="H34" s="29"/>
       <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
@@ -2560,21 +2583,21 @@
       <c r="AC34" s="8"/>
     </row>
     <row r="35">
-      <c r="A35" s="28" t="s">
-        <v>116</v>
+      <c r="A35" s="16" t="s">
+        <v>115</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24" t="s">
         <v>118</v>
-      </c>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29" t="s">
-        <v>119</v>
       </c>
       <c r="I35" s="8"/>
       <c r="J35" s="8"/>
@@ -2600,20 +2623,20 @@
     </row>
     <row r="36">
       <c r="A36" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>122</v>
+      <c r="E36" s="31" t="s">
+        <v>120</v>
       </c>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24" t="s">
-        <v>123</v>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31" t="s">
+        <v>121</v>
       </c>
       <c r="I36" s="8"/>
       <c r="J36" s="8"/>
@@ -2637,23 +2660,24 @@
       <c r="AB36" s="8"/>
       <c r="AC36" s="8"/>
     </row>
-    <row r="37" ht="105.75" customHeight="1">
-      <c r="A37" s="30" t="s">
-        <v>124</v>
+    <row r="37">
+      <c r="A37" s="32" t="s">
+        <v>122</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
-      <c r="F37" s="16"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="32"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
@@ -2676,28 +2700,22 @@
       <c r="AC37" s="8"/>
     </row>
     <row r="38" ht="105.75" customHeight="1">
-      <c r="A38" s="30" t="s">
-        <v>124</v>
+      <c r="A38" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E38" s="24"/>
-      <c r="F38" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="H38" s="24" t="s">
+      <c r="E38" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="I38" s="32" t="s">
-        <v>129</v>
-      </c>
+      <c r="F38" s="16"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="34"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
@@ -2720,11 +2738,11 @@
       <c r="AC38" s="8"/>
     </row>
     <row r="39" ht="105.75" customHeight="1">
-      <c r="A39" s="30" t="s">
-        <v>124</v>
+      <c r="A39" s="32" t="s">
+        <v>126</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>30</v>
@@ -2734,13 +2752,13 @@
         <v>31</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
-      <c r="I39" s="32" t="s">
-        <v>129</v>
+      <c r="I39" s="34" t="s">
+        <v>131</v>
       </c>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
@@ -2763,23 +2781,29 @@
       <c r="AB39" s="8"/>
       <c r="AC39" s="8"/>
     </row>
-    <row r="40">
-      <c r="A40" s="30" t="s">
+    <row r="40" ht="105.75" customHeight="1">
+      <c r="A40" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E40" s="24"/>
+      <c r="F40" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H40" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="6" t="s">
+      <c r="I40" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="G40" s="33"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="8"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -2802,26 +2826,21 @@
       <c r="AC40" s="8"/>
     </row>
     <row r="41">
-      <c r="A41" s="30" t="s">
-        <v>130</v>
+      <c r="A41" s="32" t="s">
+        <v>132</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="H41" s="25" t="s">
+      <c r="E41" s="24" t="s">
         <v>134</v>
       </c>
+      <c r="G41" s="35"/>
+      <c r="H41" s="25"/>
       <c r="I41" s="8"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2845,22 +2864,25 @@
       <c r="AC41" s="8"/>
     </row>
     <row r="42">
-      <c r="A42" s="30" t="s">
-        <v>135</v>
+      <c r="A42" s="32" t="s">
+        <v>132</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
-      <c r="E42" s="24" t="s">
-        <v>137</v>
+      <c r="E42" s="24"/>
+      <c r="F42" s="22" t="s">
+        <v>31</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24" t="s">
-        <v>138</v>
+      <c r="G42" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="H42" s="25" t="s">
+        <v>136</v>
       </c>
       <c r="I42" s="8"/>
       <c r="J42" s="8"/>
@@ -2885,30 +2907,27 @@
       <c r="AC42" s="8"/>
     </row>
     <row r="43">
-      <c r="A43" s="24" t="s">
-        <v>139</v>
+      <c r="A43" s="32" t="s">
+        <v>137</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
-      <c r="F43" s="26"/>
       <c r="G43" s="24"/>
-      <c r="H43" s="25" t="s">
-        <v>142</v>
+      <c r="H43" s="24" t="s">
+        <v>140</v>
       </c>
-      <c r="I43" s="24" t="s">
-        <v>143</v>
-      </c>
-      <c r="J43" s="35"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
       <c r="O43" s="8"/>
@@ -2929,22 +2948,26 @@
     </row>
     <row r="44">
       <c r="A44" s="24" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B44" s="11"/>
-      <c r="C44" s="4" t="s">
-        <v>145</v>
+      <c r="C44" s="6" t="s">
+        <v>142</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E44" s="24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F44" s="26"/>
       <c r="G44" s="24"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="H44" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="I44" s="24" t="s">
+        <v>145</v>
+      </c>
       <c r="J44" s="37"/>
       <c r="K44" s="11"/>
       <c r="L44" s="11"/>
@@ -2968,27 +2991,23 @@
     </row>
     <row r="45">
       <c r="A45" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="24" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F45" s="26"/>
       <c r="G45" s="24"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="J45" s="37" t="s">
-        <v>151</v>
-      </c>
+      <c r="H45" s="38"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
       <c r="K45" s="11"/>
       <c r="L45" s="11"/>
       <c r="M45" s="8"/>
@@ -3011,25 +3030,27 @@
     </row>
     <row r="46">
       <c r="A46" s="24" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B46" s="11"/>
       <c r="C46" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F46" s="26"/>
       <c r="G46" s="24"/>
-      <c r="H46" s="24" t="s">
-        <v>155</v>
+      <c r="H46" s="38"/>
+      <c r="I46" s="39" t="s">
+        <v>152</v>
       </c>
-      <c r="I46" s="35"/>
-      <c r="J46" s="35"/>
+      <c r="J46" s="39" t="s">
+        <v>153</v>
+      </c>
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>
       <c r="M46" s="8"/>
@@ -3052,27 +3073,25 @@
     </row>
     <row r="47">
       <c r="A47" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F47" s="26"/>
       <c r="G47" s="24"/>
       <c r="H47" s="24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
-      <c r="I47" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="J47" s="35"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="8"/>
@@ -3095,25 +3114,27 @@
     </row>
     <row r="48">
       <c r="A48" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F48" s="26"/>
       <c r="G48" s="24"/>
       <c r="H48" s="24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
-      <c r="I48" s="35"/>
-      <c r="J48" s="35"/>
+      <c r="I48" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="J48" s="37"/>
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
       <c r="M48" s="8"/>
@@ -3136,27 +3157,25 @@
     </row>
     <row r="49">
       <c r="A49" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F49" s="26"/>
       <c r="G49" s="24"/>
-      <c r="H49" s="25" t="s">
-        <v>168</v>
+      <c r="H49" s="24" t="s">
+        <v>166</v>
       </c>
-      <c r="I49" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="J49" s="11"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
       <c r="M49" s="8"/>
@@ -3179,22 +3198,26 @@
     </row>
     <row r="50">
       <c r="A50" s="24" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F50" s="26"/>
       <c r="G50" s="24"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="24"/>
+      <c r="H50" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="J50" s="11"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11"/>
@@ -3217,18 +3240,26 @@
       <c r="AC50" s="8"/>
     </row>
     <row r="51">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
+      <c r="A51" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="F51" s="26"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
       <c r="O51" s="8"/>
@@ -33131,8 +33162,39 @@
       <c r="AB1015" s="8"/>
       <c r="AC1015" s="8"/>
     </row>
+    <row r="1016">
+      <c r="A1016" s="8"/>
+      <c r="B1016" s="8"/>
+      <c r="C1016" s="8"/>
+      <c r="D1016" s="8"/>
+      <c r="E1016" s="8"/>
+      <c r="F1016" s="8"/>
+      <c r="G1016" s="11"/>
+      <c r="H1016" s="11"/>
+      <c r="I1016" s="8"/>
+      <c r="J1016" s="8"/>
+      <c r="K1016" s="8"/>
+      <c r="L1016" s="8"/>
+      <c r="M1016" s="8"/>
+      <c r="N1016" s="8"/>
+      <c r="O1016" s="8"/>
+      <c r="P1016" s="8"/>
+      <c r="Q1016" s="8"/>
+      <c r="R1016" s="8"/>
+      <c r="S1016" s="8"/>
+      <c r="T1016" s="8"/>
+      <c r="U1016" s="8"/>
+      <c r="V1016" s="8"/>
+      <c r="W1016" s="8"/>
+      <c r="X1016" s="8"/>
+      <c r="Y1016" s="8"/>
+      <c r="Z1016" s="8"/>
+      <c r="AA1016" s="8"/>
+      <c r="AB1016" s="8"/>
+      <c r="AC1016" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$D$1:$D$1015"/>
+  <autoFilter ref="$D$1:$D$1016"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G7"/>
     <hyperlink r:id="rId2" ref="G8"/>
@@ -33144,13 +33206,14 @@
     <hyperlink r:id="rId8" ref="G29"/>
     <hyperlink r:id="rId9" ref="G31"/>
     <hyperlink r:id="rId10" ref="E33"/>
-    <hyperlink r:id="rId11" ref="G38"/>
+    <hyperlink r:id="rId11" ref="G34"/>
     <hyperlink r:id="rId12" ref="G39"/>
-    <hyperlink r:id="rId13" ref="G41"/>
-    <hyperlink r:id="rId14" ref="I45"/>
-    <hyperlink r:id="rId15" ref="J45"/>
+    <hyperlink r:id="rId13" ref="G40"/>
+    <hyperlink r:id="rId14" ref="G42"/>
+    <hyperlink r:id="rId15" ref="I46"/>
+    <hyperlink r:id="rId16" ref="J46"/>
   </hyperlinks>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add remote datasource 1
</commit_message>
<xml_diff>
--- a/Tips web studio.xlsx
+++ b/Tips web studio.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="Feuille 2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1017</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$D$1:$D$1018</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="171">
   <si>
     <t>Ignored functional key</t>
   </si>
@@ -463,6 +463,9 @@
 [Entity Selection class](https://developer.4d.com/docs/en/ORDA/ordaClasses.html#entityselection-class)
 To learn more about datasources, visit the [documentation](https://developer.4d.com/4d-web-studio/docs/datasources/)
 and watch the tips.</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/embed/f6b3eIaYgNw</t>
   </si>
   <si>
     <t>https://www.youtube.com/embed/clGXvsHC9cQ</t>
@@ -2675,21 +2678,22 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="28"/>
+      <c r="F37" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G37" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26" t="s">
-        <v>117</v>
-      </c>
+      <c r="H37" s="26"/>
       <c r="I37" s="8"/>
       <c r="J37" s="8"/>
       <c r="K37" s="8"/>
@@ -2713,21 +2717,21 @@
       <c r="AC37" s="8"/>
     </row>
     <row r="38">
-      <c r="A38" s="33" t="s">
-        <v>118</v>
+      <c r="A38" s="18" t="s">
+        <v>115</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E38" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G38" s="26"/>
       <c r="H38" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
@@ -2751,23 +2755,24 @@
       <c r="AB38" s="8"/>
       <c r="AC38" s="8"/>
     </row>
-    <row r="39" ht="105.75" customHeight="1">
+    <row r="39">
       <c r="A39" s="33" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E39" s="26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
-      <c r="F39" s="18"/>
-      <c r="G39" s="34"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="35"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="I39" s="8"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -2791,27 +2796,21 @@
     </row>
     <row r="40" ht="105.75" customHeight="1">
       <c r="A40" s="33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E40" s="28"/>
-      <c r="F40" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G40" s="19" t="s">
+      <c r="E40" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="H40" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="I40" s="35" t="s">
-        <v>127</v>
-      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="35"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
@@ -2835,10 +2834,10 @@
     </row>
     <row r="41" ht="105.75" customHeight="1">
       <c r="A41" s="33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>30</v>
@@ -2848,13 +2847,13 @@
         <v>31</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>53</v>
+        <v>126</v>
       </c>
       <c r="H41" s="26" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="I41" s="35" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
@@ -2877,23 +2876,29 @@
       <c r="AB41" s="8"/>
       <c r="AC41" s="8"/>
     </row>
-    <row r="42">
+    <row r="42" ht="105.75" customHeight="1">
       <c r="A42" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H42" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="I42" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>130</v>
-      </c>
-      <c r="G42" s="36"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -2917,25 +2922,20 @@
     </row>
     <row r="43">
       <c r="A43" s="33" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
-      <c r="E43" s="28"/>
-      <c r="F43" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G43" s="37" t="s">
+      <c r="E43" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="H43" s="27" t="s">
-        <v>132</v>
-      </c>
+      <c r="G43" s="36"/>
+      <c r="H43" s="27"/>
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="8"/>
@@ -2960,21 +2960,24 @@
     </row>
     <row r="44">
       <c r="A44" s="33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="6" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>135</v>
+      <c r="E44" s="28"/>
+      <c r="F44" s="24" t="s">
+        <v>31</v>
       </c>
-      <c r="G44" s="26"/>
-      <c r="H44" s="26" t="s">
-        <v>136</v>
+      <c r="G44" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="H44" s="27" t="s">
+        <v>133</v>
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="8"/>
@@ -2999,30 +3002,27 @@
       <c r="AC44" s="8"/>
     </row>
     <row r="45">
-      <c r="A45" s="26" t="s">
-        <v>137</v>
+      <c r="A45" s="33" t="s">
+        <v>134</v>
       </c>
-      <c r="B45" s="11"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E45" s="26" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
-      <c r="F45" s="29"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="27" t="s">
-        <v>140</v>
+      <c r="H45" s="26" t="s">
+        <v>137</v>
       </c>
-      <c r="I45" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="J45" s="38"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+      <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
       <c r="O45" s="8"/>
@@ -3043,23 +3043,27 @@
     </row>
     <row r="46">
       <c r="A46" s="26" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B46" s="11"/>
-      <c r="C46" s="4" t="s">
-        <v>143</v>
+      <c r="C46" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="26" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F46" s="29"/>
       <c r="G46" s="26"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="40"/>
+      <c r="H46" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="J46" s="38"/>
       <c r="K46" s="11"/>
       <c r="L46" s="11"/>
       <c r="M46" s="8"/>
@@ -3082,27 +3086,23 @@
     </row>
     <row r="47">
       <c r="A47" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E47" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" s="26"/>
       <c r="H47" s="39"/>
-      <c r="I47" s="40" t="s">
-        <v>148</v>
-      </c>
-      <c r="J47" s="40" t="s">
-        <v>149</v>
-      </c>
+      <c r="I47" s="40"/>
+      <c r="J47" s="40"/>
       <c r="K47" s="11"/>
       <c r="L47" s="11"/>
       <c r="M47" s="8"/>
@@ -3125,25 +3125,27 @@
     </row>
     <row r="48">
       <c r="A48" s="26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B48" s="11"/>
       <c r="C48" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F48" s="29"/>
       <c r="G48" s="26"/>
-      <c r="H48" s="26" t="s">
-        <v>153</v>
+      <c r="H48" s="39"/>
+      <c r="I48" s="40" t="s">
+        <v>149</v>
       </c>
-      <c r="I48" s="38"/>
-      <c r="J48" s="38"/>
+      <c r="J48" s="40" t="s">
+        <v>150</v>
+      </c>
       <c r="K48" s="11"/>
       <c r="L48" s="11"/>
       <c r="M48" s="8"/>
@@ -3166,26 +3168,24 @@
     </row>
     <row r="49">
       <c r="A49" s="26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B49" s="11"/>
       <c r="C49" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F49" s="29"/>
       <c r="G49" s="26"/>
       <c r="H49" s="26" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
-      <c r="I49" s="26" t="s">
-        <v>158</v>
-      </c>
+      <c r="I49" s="38"/>
       <c r="J49" s="38"/>
       <c r="K49" s="11"/>
       <c r="L49" s="11"/>
@@ -3209,24 +3209,26 @@
     </row>
     <row r="50">
       <c r="A50" s="26" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B50" s="11"/>
       <c r="C50" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F50" s="29"/>
       <c r="G50" s="26"/>
       <c r="H50" s="26" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
-      <c r="I50" s="38"/>
+      <c r="I50" s="26" t="s">
+        <v>159</v>
+      </c>
       <c r="J50" s="38"/>
       <c r="K50" s="11"/>
       <c r="L50" s="11"/>
@@ -3250,27 +3252,25 @@
     </row>
     <row r="51">
       <c r="A51" s="26" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B51" s="11"/>
       <c r="C51" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F51" s="29"/>
       <c r="G51" s="26"/>
-      <c r="H51" s="27" t="s">
-        <v>166</v>
+      <c r="H51" s="26" t="s">
+        <v>163</v>
       </c>
-      <c r="I51" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="J51" s="11"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="38"/>
       <c r="K51" s="11"/>
       <c r="L51" s="11"/>
       <c r="M51" s="8"/>
@@ -3293,22 +3293,26 @@
     </row>
     <row r="52">
       <c r="A52" s="26" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B52" s="11"/>
       <c r="C52" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F52" s="29"/>
       <c r="G52" s="26"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="26"/>
+      <c r="H52" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="I52" s="26" t="s">
+        <v>168</v>
+      </c>
       <c r="J52" s="11"/>
       <c r="K52" s="11"/>
       <c r="L52" s="11"/>
@@ -3331,18 +3335,26 @@
       <c r="AC52" s="8"/>
     </row>
     <row r="53">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="8"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="8"/>
+      <c r="A53" s="26" t="s">
+        <v>164</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="F53" s="29"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="26"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
       <c r="O53" s="8"/>
@@ -33245,8 +33257,39 @@
       <c r="AB1017" s="8"/>
       <c r="AC1017" s="8"/>
     </row>
+    <row r="1018">
+      <c r="A1018" s="8"/>
+      <c r="B1018" s="8"/>
+      <c r="C1018" s="8"/>
+      <c r="D1018" s="8"/>
+      <c r="E1018" s="8"/>
+      <c r="F1018" s="8"/>
+      <c r="G1018" s="11"/>
+      <c r="H1018" s="11"/>
+      <c r="I1018" s="8"/>
+      <c r="J1018" s="8"/>
+      <c r="K1018" s="8"/>
+      <c r="L1018" s="8"/>
+      <c r="M1018" s="8"/>
+      <c r="N1018" s="8"/>
+      <c r="O1018" s="8"/>
+      <c r="P1018" s="8"/>
+      <c r="Q1018" s="8"/>
+      <c r="R1018" s="8"/>
+      <c r="S1018" s="8"/>
+      <c r="T1018" s="8"/>
+      <c r="U1018" s="8"/>
+      <c r="V1018" s="8"/>
+      <c r="W1018" s="8"/>
+      <c r="X1018" s="8"/>
+      <c r="Y1018" s="8"/>
+      <c r="Z1018" s="8"/>
+      <c r="AA1018" s="8"/>
+      <c r="AB1018" s="8"/>
+      <c r="AC1018" s="8"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$D$1:$D$1017"/>
+  <autoFilter ref="$D$1:$D$1018"/>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="G7"/>
     <hyperlink r:id="rId2" ref="G8"/>
@@ -33260,13 +33303,14 @@
     <hyperlink r:id="rId10" ref="G32"/>
     <hyperlink r:id="rId11" ref="E34"/>
     <hyperlink r:id="rId12" ref="G36"/>
-    <hyperlink r:id="rId13" ref="G40"/>
+    <hyperlink r:id="rId13" ref="G37"/>
     <hyperlink r:id="rId14" ref="G41"/>
-    <hyperlink r:id="rId15" ref="G43"/>
-    <hyperlink r:id="rId16" ref="I47"/>
-    <hyperlink r:id="rId17" ref="J47"/>
+    <hyperlink r:id="rId15" ref="G42"/>
+    <hyperlink r:id="rId16" ref="G44"/>
+    <hyperlink r:id="rId17" ref="I48"/>
+    <hyperlink r:id="rId18" ref="J48"/>
   </hyperlinks>
-  <drawing r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>